<commit_message>
Sprint 2 70% -- Sprint 3 30%
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\Cursos\Cursos_2025\2025-02\Proyecto - 2\CARPETAS\TALLER_DE_PROYECTOS_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{966E3103-E6CB-48A2-A4A6-76337131A8B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A99735D-7C68-44F7-9A06-D0A4D1640222}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8076" activeTab="3" xr2:uid="{DFE89E42-E55B-4B7D-89EA-0CD2B781E058}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8076" activeTab="2" xr2:uid="{DFE89E42-E55B-4B7D-89EA-0CD2B781E058}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 " sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_Hlk210578957" localSheetId="1">'Sprint 2 '!$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="79">
   <si>
     <t>HU ID</t>
   </si>
@@ -259,6 +260,15 @@
   </si>
   <si>
     <t>Todos</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>Esperado</t>
+  </si>
+  <si>
+    <t>Estimado</t>
   </si>
 </sst>
 </file>
@@ -399,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -477,6 +487,12 @@
     <xf numFmtId="14" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,6 +508,3150 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PE"/>
+              <a:t>Burdown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-PE" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1 '!$G$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Esperado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$F$17:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45905</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45906</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45908</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$G$17:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F64A-4F6C-8C77-63B2DC5691D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1 '!$H$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$F$17:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45905</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45906</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45908</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$H$17:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F64A-4F6C-8C77-63B2DC5691D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="80935120"/>
+        <c:axId val="74229792"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="80935120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74229792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="74229792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="80935120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PE"/>
+              <a:t>Burdown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-PE" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2 '!$F$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2 '!$E$13:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>45909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45910</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45912</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45914</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2 '!$F$13:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA0B-402F-9957-B968DBF196D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2 '!$G$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2 '!$E$13:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>45909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45910</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45912</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45914</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2 '!$G$13:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DA0B-402F-9957-B968DBF196D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="79609328"/>
+        <c:axId val="74236032"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="79609328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74236032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="74236032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79609328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PE"/>
+              <a:t>Burdown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-PE" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 3 '!$F$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 3 '!$E$14:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>45915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45916</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45917</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3 '!$F$14:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DC9-44D9-ACA7-476825F9B542}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 3 '!$G$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 3 '!$E$14:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>45915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45916</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45917</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45919</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3 '!$G$14:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9DC9-44D9-ACA7-476825F9B542}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1059880175"/>
+        <c:axId val="1252314159"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1059880175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1252314159"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1252314159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1059880175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2096518</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>24856</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>224117</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>753035</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7C919A0-EFA1-4D1F-B324-CD996BBC3626}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>90055</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>6927</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>166255</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>55417</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEEF9455-A36B-466A-9922-C53D35EA787A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>34636</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>48491</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>858982</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FB5E1CF-292A-401B-A464-99BFA7051BF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -791,9 +3951,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7005A097-3D20-45B1-8762-77FC135B0ACD}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H14" sqref="A6:H14"/>
     </sheetView>
   </sheetViews>
@@ -804,7 +3964,7 @@
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
     <col min="7" max="7" width="12.109375" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" customWidth="1"/>
   </cols>
@@ -966,7 +4126,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="22">
-        <f>+G7</f>
+        <f t="shared" ref="F8:F14" si="0">+G7</f>
         <v>45901</v>
       </c>
       <c r="G8" s="22">
@@ -994,7 +4154,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="19">
-        <f>+G8</f>
+        <f t="shared" si="0"/>
         <v>45902</v>
       </c>
       <c r="G9" s="19">
@@ -1022,7 +4182,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="22">
-        <f>+G9</f>
+        <f t="shared" si="0"/>
         <v>45903</v>
       </c>
       <c r="G10" s="22">
@@ -1050,7 +4210,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="19">
-        <f>+G10</f>
+        <f t="shared" si="0"/>
         <v>45904</v>
       </c>
       <c r="G11" s="19">
@@ -1078,7 +4238,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="22">
-        <f>+G11</f>
+        <f t="shared" si="0"/>
         <v>45905</v>
       </c>
       <c r="G12" s="22">
@@ -1106,7 +4266,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="19">
-        <f>+G12</f>
+        <f t="shared" si="0"/>
         <v>45905</v>
       </c>
       <c r="G13" s="19">
@@ -1134,7 +4294,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="22">
-        <f>+G13</f>
+        <f t="shared" si="0"/>
         <v>45906</v>
       </c>
       <c r="G14" s="22">
@@ -1145,18 +4305,254 @@
         <v>35</v>
       </c>
     </row>
+    <row r="15" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="18">
+        <v>3</v>
+      </c>
+      <c r="F17" s="19">
+        <v>45901</v>
+      </c>
+      <c r="G17" s="27">
+        <v>13</v>
+      </c>
+      <c r="H17" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="17">
+        <v>2</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="21">
+        <v>3</v>
+      </c>
+      <c r="F18" s="22">
+        <v>45902</v>
+      </c>
+      <c r="G18" s="28">
+        <v>10</v>
+      </c>
+      <c r="H18" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="17">
+        <v>3</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="18">
+        <v>2</v>
+      </c>
+      <c r="F19" s="19">
+        <v>45903</v>
+      </c>
+      <c r="G19" s="27">
+        <v>9</v>
+      </c>
+      <c r="H19" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="17">
+        <v>4</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="21">
+        <v>2</v>
+      </c>
+      <c r="F20" s="22">
+        <v>45904</v>
+      </c>
+      <c r="G20" s="28">
+        <v>8</v>
+      </c>
+      <c r="H20" s="28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="17">
+        <v>5</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="18">
+        <v>2</v>
+      </c>
+      <c r="F21" s="19">
+        <v>45905</v>
+      </c>
+      <c r="G21" s="27">
+        <v>6</v>
+      </c>
+      <c r="H21" s="27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17">
+        <v>6</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="21">
+        <v>3</v>
+      </c>
+      <c r="F22" s="22">
+        <v>45905</v>
+      </c>
+      <c r="G22" s="28">
+        <v>3</v>
+      </c>
+      <c r="H22" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="17">
+        <v>7</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="18">
+        <v>4</v>
+      </c>
+      <c r="F23" s="19">
+        <v>45906</v>
+      </c>
+      <c r="G23" s="27">
+        <v>2</v>
+      </c>
+      <c r="H23" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="17">
+        <v>8</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="21">
+        <v>3</v>
+      </c>
+      <c r="F24" s="22">
+        <v>45908</v>
+      </c>
+      <c r="G24" s="28">
+        <v>0</v>
+      </c>
+      <c r="H24" s="28">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7AD805-9F79-482F-9894-2D3904CEEE57}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,14 +4560,13 @@
     <col min="1" max="1" width="8.77734375" style="23" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="23" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="7" width="15.44140625" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="55.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +4586,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="97.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="17" t="s">
         <v>36</v>
       </c>
@@ -1380,17 +4775,157 @@
         <v>47</v>
       </c>
     </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="17">
+        <v>9</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="19">
+        <v>45909</v>
+      </c>
+      <c r="F13" s="18">
+        <v>22</v>
+      </c>
+      <c r="G13" s="18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="17">
+        <v>10</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="22">
+        <v>45910</v>
+      </c>
+      <c r="F14" s="21">
+        <v>18</v>
+      </c>
+      <c r="G14" s="21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="17">
+        <v>11</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="19">
+        <v>45912</v>
+      </c>
+      <c r="F15" s="18">
+        <v>14</v>
+      </c>
+      <c r="G15" s="18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="17">
+        <v>12</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="22">
+        <v>45914</v>
+      </c>
+      <c r="F16" s="21">
+        <v>8</v>
+      </c>
+      <c r="G16" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="19">
+        <v>45915</v>
+      </c>
+      <c r="F17" s="18">
+        <v>0</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4928B1D4-B006-4047-964D-C09CD7DEA272}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.33203125" defaultRowHeight="46.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1400,8 +4935,8 @@
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
     <col min="8" max="8" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1664,8 +5199,176 @@
         <v>61</v>
       </c>
     </row>
+    <row r="12" spans="1:8" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:8" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="12">
+        <v>45915</v>
+      </c>
+      <c r="F14" s="5">
+        <f>+SUM(E6:E11)</f>
+        <v>22</v>
+      </c>
+      <c r="G14" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>15</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="11">
+        <v>45916</v>
+      </c>
+      <c r="F15" s="6">
+        <f>+F14-E6</f>
+        <v>19</v>
+      </c>
+      <c r="G15" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="12">
+        <v>45917</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" ref="F16:F19" si="0">+F15-E7</f>
+        <v>15</v>
+      </c>
+      <c r="G16" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>17</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="11">
+        <v>45919</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G17" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="12">
+        <v>45921</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G18" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>19</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="11">
+        <v>45922</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1673,8 +5376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1AFC42-F163-4781-B91C-41AD7CBCCCE1}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H11" sqref="A5:H11"/>
+    <sheetView topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Sprint 1 : 100 %
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\Cursos\Cursos_2025\2025-02\Proyecto - 2\CARPETAS\TALLER_DE_PROYECTOS_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E9EB94-E42A-4E24-B001-BD3A27710AEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3964509-2B23-4B89-8098-F2D9C78E88B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8076" activeTab="5" xr2:uid="{DFE89E42-E55B-4B7D-89EA-0CD2B781E058}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8076" xr2:uid="{DFE89E42-E55B-4B7D-89EA-0CD2B781E058}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 " sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="152">
   <si>
     <t>Historia de Usuario</t>
   </si>
@@ -450,12 +450,69 @@
   <si>
     <t>Experiencia de usuario y entrega final</t>
   </si>
+  <si>
+    <t>HU-1</t>
+  </si>
+  <si>
+    <t>HU-2</t>
+  </si>
+  <si>
+    <t>HU-3</t>
+  </si>
+  <si>
+    <t>Diseñar esquema de BD para usuarios y roles</t>
+  </si>
+  <si>
+    <t>Implementar autenticación (Login/Register)</t>
+  </si>
+  <si>
+    <t>Configurar controladores y rutas en backend</t>
+  </si>
+  <si>
+    <t>Crear interfaz de registro y login</t>
+  </si>
+  <si>
+    <t>Pruebas de seguridad y sesión</t>
+  </si>
+  <si>
+    <t>Crear consultas SQL de resumen</t>
+  </si>
+  <si>
+    <t>Implementar dashboard con métricas (usuarios activos, progreso)</t>
+  </si>
+  <si>
+    <t>Conectar con frontend (gráficos dinámicos)</t>
+  </si>
+  <si>
+    <t>Crear script de backup automático de BD</t>
+  </si>
+  <si>
+    <t>Integrar restauración manual desde panel admin</t>
+  </si>
+  <si>
+    <t>Pruebas de recuperación de datos</t>
+  </si>
+  <si>
+    <t>TAREAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPRINT 1 </t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>Esperado</t>
+  </si>
+  <si>
+    <t>Real2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,16 +533,36 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -493,11 +570,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -520,11 +672,87 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="77">
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -545,25 +773,25 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -625,16 +853,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -699,16 +926,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -774,14 +1000,17 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -809,15 +1038,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -845,18 +1075,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -884,15 +1111,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -919,23 +1147,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -949,66 +1160,1072 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PE"/>
+              <a:t>BURNDOWN CHART</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1 '!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Esperado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45934</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45939</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45956</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7049-4871-AA35-DAB1A4979080}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1 '!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>45934</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45939</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45956</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1 '!$G$2:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7049-4871-AA35-DAB1A4979080}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1258400896"/>
+        <c:axId val="1260183872"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1258400896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1260183872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1260183872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1258400896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1850572</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>59872</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>511629</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>234043</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C40B3550-E95D-4F8D-9F45-D0EAD79A743E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BD16BBC-76A7-4CBA-BD96-3B16F878E2EB}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0" headerRowDxfId="69">
-  <autoFilter ref="A1:E4" xr:uid="{24F748EC-318B-4855-BCC0-0DBC9C8A5746}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E093E692-05C3-4735-978E-D768DE69C78D}" name="Historias de Usuario" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{35C8A382-20E4-445F-9C96-2559CD04C663}" name="Observaciones" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{97627D17-1AAA-478F-9A9E-B47AC1BBD346}" name="Puntos" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{D6D7A7D7-9517-47B1-8D78-05F39A8C7B28}" name="Inicio" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{28F7D3BC-9628-49BE-9C4B-6275D6B13920}" name="Fin" dataDxfId="70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BD16BBC-76A7-4CBA-BD96-3B16F878E2EB}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:G4" xr:uid="{24F748EC-318B-4855-BCC0-0DBC9C8A5746}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E093E692-05C3-4735-978E-D768DE69C78D}" name="Historias de Usuario" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{35C8A382-20E4-445F-9C96-2559CD04C663}" name="Observaciones" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{D6D7A7D7-9517-47B1-8D78-05F39A8C7B28}" name="Inicio" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{28F7D3BC-9628-49BE-9C4B-6275D6B13920}" name="Fin" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{988F7153-31B6-4665-B292-DD1835FCA682}" name="Real" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{97627D17-1AAA-478F-9A9E-B47AC1BBD346}" name="Esperado" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{06B6D843-3508-4C54-AF98-79F0B9E21D5E}" name="Real2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A5E22D20-0412-4B20-B6F6-E20FCAE65091}" name="Table11" displayName="Table11" ref="H1:L7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A5E22D20-0412-4B20-B6F6-E20FCAE65091}" name="Table11" displayName="Table11" ref="H1:L7" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="H1:L7" xr:uid="{C396598D-C1B2-4EDD-96A4-689190CBEF86}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{28EE093D-5249-49C9-B6A0-1FD25097DE2A}" name="ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{FA6D1229-FD84-4D2A-813A-2AEA4E6BEAC3}" name="Historia de Usuario" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{E5454D72-00EF-427B-9AED-6F323451CBB2}" name="Tareas / Actividades" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{D2518746-B270-4548-868C-AE977DC56C2A}" name="Responsable" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{65FE5E18-EB2E-4BC9-BACE-5606BAF908C7}" name="Estado" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{28EE093D-5249-49C9-B6A0-1FD25097DE2A}" name="ID" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{FA6D1229-FD84-4D2A-813A-2AEA4E6BEAC3}" name="Historia de Usuario" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{E5454D72-00EF-427B-9AED-6F323451CBB2}" name="Tareas / Actividades" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{D2518746-B270-4548-868C-AE977DC56C2A}" name="Responsable" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{65FE5E18-EB2E-4BC9-BACE-5606BAF908C7}" name="Estado" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D0FE58DA-BDB6-4A7A-ABD0-C1BCE573E051}" name="Table12" displayName="Table12" ref="A1:G6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D0FE58DA-BDB6-4A7A-ABD0-C1BCE573E051}" name="Table12" displayName="Table12" ref="A1:G6" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:G6" xr:uid="{36140BD1-2857-4354-99CF-65B2C864054D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A3ECDFC0-0119-4E81-8248-735E24E3A50C}" name="Sprint" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{90220717-9109-4AC8-A400-0997D4D01066}" name="Épica" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{98DAC554-28EE-4D24-BB44-681616A59DB1}" name="Historias" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{57F5AACE-D807-4B9A-99E2-35CB3A260C48}" name="Tareas promedio" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{972F0FF7-7B5C-457D-B9AA-BC30C5C99195}" name="Puntos totales" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{260E1B46-1DCC-4DE4-90EE-1DA31F556276}" name="Duración" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{5B2A6FB1-2AE1-4691-B744-886702761CF2}" name="Objetivo" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A3ECDFC0-0119-4E81-8248-735E24E3A50C}" name="Sprint" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{90220717-9109-4AC8-A400-0997D4D01066}" name="Épica" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{98DAC554-28EE-4D24-BB44-681616A59DB1}" name="Historias" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{57F5AACE-D807-4B9A-99E2-35CB3A260C48}" name="Tareas promedio" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{972F0FF7-7B5C-457D-B9AA-BC30C5C99195}" name="Puntos totales" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{260E1B46-1DCC-4DE4-90EE-1DA31F556276}" name="Duración" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{5B2A6FB1-2AE1-4691-B744-886702761CF2}" name="Objetivo" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0D7FE01E-8BFD-4557-8ABB-277B2D16BD1D}" name="Table7" displayName="Table7" ref="H1:L4" totalsRowShown="0" headerRowDxfId="37" dataDxfId="38">
-  <autoFilter ref="H1:L4" xr:uid="{57F0D9A7-1F1F-4171-8A4B-62F309C48136}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0D7FE01E-8BFD-4557-8ABB-277B2D16BD1D}" name="Table7" displayName="Table7" ref="J1:N4" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+  <autoFilter ref="J1:N4" xr:uid="{57F0D9A7-1F1F-4171-8A4B-62F309C48136}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BEA83294-6A18-42BB-B11B-0502438CC099}" name="ID" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{1A33C792-A304-4AE5-9F2D-C3BAC8C06183}" name="Historia de Usuario" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{BF3DAA27-8C45-4CFF-B21D-90A5DA20614E}" name="Tareas / Actividades Técnicas" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{FEBBCEB6-57C5-4054-AFF3-09743B4D7B77}" name="Responsable" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{2655B592-AE60-4AF0-8400-A491855DABCF}" name="Estado" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{BEA83294-6A18-42BB-B11B-0502438CC099}" name="ID" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{1A33C792-A304-4AE5-9F2D-C3BAC8C06183}" name="Historia de Usuario" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{BF3DAA27-8C45-4CFF-B21D-90A5DA20614E}" name="Tareas / Actividades Técnicas" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{FEBBCEB6-57C5-4054-AFF3-09743B4D7B77}" name="Responsable" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{2655B592-AE60-4AF0-8400-A491855DABCF}" name="Estado" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86670D76-0C19-48B7-8C69-376882E9C5A5}" name="Table3" displayName="Table3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{86670D76-0C19-48B7-8C69-376882E9C5A5}" name="Table3" displayName="Table3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="69">
   <autoFilter ref="A1:E4" xr:uid="{E46CBD97-9127-4EC7-A76C-6EB5EBAE965A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BA6DF882-EE40-476C-9EFC-3133B0684925}" name="Historias de Usuario" dataDxfId="68"/>
@@ -1022,84 +2239,84 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B8C64535-8DAD-46AF-A834-BCDC56173B9E}" name="Table8" displayName="Table8" ref="G1:K4" totalsRowShown="0" headerRowDxfId="30" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B8C64535-8DAD-46AF-A834-BCDC56173B9E}" name="Table8" displayName="Table8" ref="G1:K4" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="G1:K4" xr:uid="{AB1E57C0-467F-44F0-B371-05901AFD95F2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{22AF7A06-F85C-4498-9E50-6A63E63B44B3}" name="ID" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{BFA8754B-9EFF-426F-9E72-CE4B22401BF3}" name="Historia" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{9970E561-8A84-41BD-AF63-40C524209079}" name="Tareas / Actividades" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{DC12B0AC-B9A6-4F10-9BFC-C1290A58EC33}" name="Responsable" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{946E27B7-2113-4FBD-B903-F96D85DB6542}" name="Estado" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{22AF7A06-F85C-4498-9E50-6A63E63B44B3}" name="ID" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{BFA8754B-9EFF-426F-9E72-CE4B22401BF3}" name="Historia" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{9970E561-8A84-41BD-AF63-40C524209079}" name="Tareas / Actividades" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{DC12B0AC-B9A6-4F10-9BFC-C1290A58EC33}" name="Responsable" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{946E27B7-2113-4FBD-B903-F96D85DB6542}" name="Estado" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1ADFA7C0-8565-4A68-8322-B63EC9B18BF9}" name="Table4" displayName="Table4" ref="A1:E5" totalsRowShown="0" headerRowDxfId="56" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1ADFA7C0-8565-4A68-8322-B63EC9B18BF9}" name="Table4" displayName="Table4" ref="A1:E5" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A1:E5" xr:uid="{3A0FA1D2-2F09-414E-A712-1DD789816677}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D3A42CD4-A8D1-4AAD-B723-77E241709C9F}" name="Historias de Usuario" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{A7101206-0493-4473-B3A0-F64FB9ED81D4}" name="Observaciones" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{69BC9BCF-3433-451E-923D-B29AF2B0C3B0}" name="Puntos" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{BCBD9DC0-9F99-4885-8F6A-616E3EA9344E}" name="Inicio" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{1961FEF6-E92E-44D1-A7A7-4F9976DDF655}" name="Fin" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{D3A42CD4-A8D1-4AAD-B723-77E241709C9F}" name="Historias de Usuario" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{A7101206-0493-4473-B3A0-F64FB9ED81D4}" name="Observaciones" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{69BC9BCF-3433-451E-923D-B29AF2B0C3B0}" name="Puntos" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{BCBD9DC0-9F99-4885-8F6A-616E3EA9344E}" name="Inicio" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{1961FEF6-E92E-44D1-A7A7-4F9976DDF655}" name="Fin" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{597891A9-4490-41DE-B6B6-27BF9D57E64A}" name="Table9" displayName="Table9" ref="I1:M5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{597891A9-4490-41DE-B6B6-27BF9D57E64A}" name="Table9" displayName="Table9" ref="I1:M5" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="I1:M5" xr:uid="{6EA5FF5D-303B-47DA-8671-AA9BDBBE3AB1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D38AB8C0-6910-4139-99CE-23B6526AB348}" name="ID" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{49E76221-10CE-49C3-B206-98486DE47326}" name="Historia de Usuario" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{25DF9D1B-DD40-4AD6-AE21-71BD43D3B2BE}" name="Tareas / Actividades" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{1D59739A-6AD8-40F3-8EF1-8071A3600036}" name="Responsable" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{E25EDDE4-F757-4E99-93D1-3F20D175D9BF}" name="Estado" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{D38AB8C0-6910-4139-99CE-23B6526AB348}" name="ID" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{49E76221-10CE-49C3-B206-98486DE47326}" name="Historia de Usuario" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{25DF9D1B-DD40-4AD6-AE21-71BD43D3B2BE}" name="Tareas / Actividades" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{1D59739A-6AD8-40F3-8EF1-8071A3600036}" name="Responsable" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{E25EDDE4-F757-4E99-93D1-3F20D175D9BF}" name="Estado" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4C0CAFD9-DCBA-4C79-87F4-27B771AF5505}" name="Table5" displayName="Table5" ref="A1:E4" totalsRowShown="0" headerRowDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4C0CAFD9-DCBA-4C79-87F4-27B771AF5505}" name="Table5" displayName="Table5" ref="A1:E4" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="A1:E4" xr:uid="{E8A03F14-0939-4B33-BA50-2E152FC11783}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2700169D-C943-4B60-8B33-90815354B35D}" name="Historias de Usuario" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{3D265D97-82AD-4E8D-BDAE-A226B79CD457}" name="Observaciones" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{5FA19ED7-47FE-4C52-9B48-98C04EDA85E7}" name="Puntos" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{B10E452E-2553-454F-B74E-6BAA647B0C0E}" name="Inicio" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{463884B4-07B7-4D83-9E8E-0FA3177ADB03}" name="Fin" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{2700169D-C943-4B60-8B33-90815354B35D}" name="Historias de Usuario" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{3D265D97-82AD-4E8D-BDAE-A226B79CD457}" name="Observaciones" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{5FA19ED7-47FE-4C52-9B48-98C04EDA85E7}" name="Puntos" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{B10E452E-2553-454F-B74E-6BAA647B0C0E}" name="Inicio" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{463884B4-07B7-4D83-9E8E-0FA3177ADB03}" name="Fin" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{81D04F5D-4DA9-4EC5-8B62-C526D1D60754}" name="Table10" displayName="Table10" ref="J1:N4" totalsRowShown="0" headerRowDxfId="16" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{81D04F5D-4DA9-4EC5-8B62-C526D1D60754}" name="Table10" displayName="Table10" ref="J1:N4" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="J1:N4" xr:uid="{8B3B822A-9D65-491D-BD34-38117E174830}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CE68E439-0EAA-4E12-A396-0E9E594FF481}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{82A6BD14-78BC-444F-9C6A-83DF22A810A2}" name="Historia de Usuario" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{B11D97D7-D383-46EF-BEB4-877A64049C20}" name="Tareas / Actividades" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{48AADF17-8EFA-4D6C-AE10-E90945A69C74}" name="Responsable" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{2AF34DCF-3760-40F2-9102-8844A5BDBD05}" name="Estado" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{CE68E439-0EAA-4E12-A396-0E9E594FF481}" name="ID" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{82A6BD14-78BC-444F-9C6A-83DF22A810A2}" name="Historia de Usuario" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B11D97D7-D383-46EF-BEB4-877A64049C20}" name="Tareas / Actividades" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{48AADF17-8EFA-4D6C-AE10-E90945A69C74}" name="Responsable" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{2AF34DCF-3760-40F2-9102-8844A5BDBD05}" name="Estado" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B5DD6B28-3BCD-4005-B2E1-456C3A701567}" name="Table6" displayName="Table6" ref="A1:E7" totalsRowShown="0" headerRowDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B5DD6B28-3BCD-4005-B2E1-456C3A701567}" name="Table6" displayName="Table6" ref="A1:E7" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:E7" xr:uid="{19214B5D-F8DC-4A15-8E72-4476E189B1D7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E98C7EF1-F8F7-4B39-9E39-578A2A8E077C}" name="Historias de Usuario" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{B80B1AC0-0334-4AEE-AA67-80DDEF410BC6}" name="Observaciones" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{87074347-A10C-4F44-94F0-60AFE6D2A979}" name="Puntos" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{FB7D837E-C528-4C63-A1E2-A1AD9203C11F}" name="Inicio" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{26C8AAA5-A94E-4A8B-8E40-D6CD8CDAC116}" name="Fin" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{E98C7EF1-F8F7-4B39-9E39-578A2A8E077C}" name="Historias de Usuario" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{B80B1AC0-0334-4AEE-AA67-80DDEF410BC6}" name="Observaciones" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{87074347-A10C-4F44-94F0-60AFE6D2A979}" name="Puntos" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{FB7D837E-C528-4C63-A1E2-A1AD9203C11F}" name="Inicio" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{26C8AAA5-A94E-4A8B-8E40-D6CD8CDAC116}" name="Fin" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1402,23 +2619,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF168A87-6B13-40AD-99BE-AE163F7E8306}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L4" sqref="H1:L4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="29.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="25"/>
+    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="29.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="19" max="20" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="57.6">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1426,131 +2649,246 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="124.8" customHeight="1">
+    <row r="2" spans="1:14" ht="124.8" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1">
-        <v>8</v>
+      <c r="C2" s="4">
+        <v>45925</v>
       </c>
       <c r="D2" s="4">
-        <v>45925</v>
+        <v>45934</v>
       </c>
       <c r="E2" s="4">
         <v>45934</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="1">
+        <v>16</v>
+      </c>
+      <c r="G2" s="23">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="J2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="124.8" customHeight="1">
+    <row r="3" spans="1:14" ht="103.8" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1">
-        <v>5</v>
+      <c r="C3" s="4">
+        <v>45925</v>
       </c>
       <c r="D3" s="4">
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="E3" s="4">
         <v>45939</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3" s="23">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="J3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="124.8" customHeight="1">
+    <row r="4" spans="1:14" ht="88.8" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
+        <v>45931</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45939</v>
+      </c>
+      <c r="E4" s="21">
+        <v>45956</v>
+      </c>
+      <c r="F4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="4">
-        <v>45931</v>
-      </c>
-      <c r="E4" s="4">
-        <v>45939</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="24">
+        <v>3</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="J4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>55</v>
       </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="J10" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="28.8">
+      <c r="J11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="57.6">
+      <c r="J12" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="57.6">
+      <c r="J13" s="19"/>
+      <c r="K13" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="43.2">
+      <c r="J14" s="19"/>
+      <c r="K14" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="28.8">
+      <c r="J15" s="19"/>
+      <c r="K15" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" ht="28.8">
+      <c r="J16" s="20"/>
+      <c r="K16" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J12:J16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1569,7 +2907,7 @@
     <col min="9" max="9" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1712,7 +3050,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:M5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1722,7 +3060,7 @@
     <col min="12" max="12" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="43.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1906,7 +3244,7 @@
     <col min="13" max="13" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="43.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -2047,7 +3385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962FA179-2D3F-4332-84D1-DDF21F5C3B71}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C6" workbookViewId="0">
       <selection activeCell="L7" sqref="H1:L7"/>
     </sheetView>
   </sheetViews>
@@ -2298,7 +3636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB58825C-42F9-4997-BB29-C8CCF1405C4D}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
@@ -2311,7 +3649,7 @@
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>113</v>
       </c>
@@ -2334,7 +3672,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2">
+    <row r="2" spans="1:7" ht="28.8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2357,7 +3695,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="72">
+    <row r="3" spans="1:7" ht="43.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2380,7 +3718,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57.6">
+    <row r="4" spans="1:7" ht="43.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2403,7 +3741,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="57.6">
+    <row r="5" spans="1:7" ht="43.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2426,7 +3764,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="72">
+    <row r="6" spans="1:7" ht="43.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>

</xml_diff>